<commit_message>
Reformatting to OOP format
</commit_message>
<xml_diff>
--- a/config/data.xlsx
+++ b/config/data.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="147">
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Product Code</t>
-  </si>
-  <si>
-    <t>Product Image URL</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Image URL</t>
   </si>
   <si>
     <t>Капуста айсберг вес</t>
@@ -806,7 +806,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>